<commit_message>
Various updates on the project
</commit_message>
<xml_diff>
--- a/trimmed_final_journals.xlsx
+++ b/trimmed_final_journals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emine\PycharmProjects\Article-Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370F2D6A-1042-4B61-956B-27D020605EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676BDFC3-DD38-4C67-9E71-C7597A5BBDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="1158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1789" uniqueCount="1159">
   <si>
     <t xml:space="preserve"> Abant Sağlık Bilimleri ve Teknolojileri Dergisi </t>
   </si>
@@ -3502,6 +3502,9 @@
   </si>
   <si>
     <t>MINI</t>
+  </si>
+  <si>
+    <t>ejgg dergisi aslında bu dergi</t>
   </si>
 </sst>
 </file>
@@ -3839,8 +3842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F569"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4108,6 +4111,9 @@
       </c>
       <c r="C20" t="s">
         <v>761</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1158</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>